<commit_message>
Added in displayed author for main list
</commit_message>
<xml_diff>
--- a/sample-posts-analyzed.xlsx
+++ b/sample-posts-analyzed.xlsx
@@ -368,13 +368,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="20.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1">
@@ -385,30 +385,35 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>date</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>yoast_metadesc</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>excerpt</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>category</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>tags</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>url_path</t>
         </is>
@@ -419,30 +424,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/our-devops-toolbox-consul/","Our DevOps Toolbox: Consul")</f>
         <v>0</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Exadel Digital Transformation Team</t>
+        </is>
+      </c>
+      <c r="C2" s="3">
         <v>43819</v>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Consul provides service discovery, health checks, load balancing &amp; key/value storage for services &amp; applications. Find out the benefits we've seen using it.</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>Consul provides service discovery, health checks, load balancing and key/value storage for services and applications. Find out the benefits we've seen using it for development and business.</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>Tools</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>Consul,DevOps,devopstoolbox series,digital transformation,series</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>/news/our-devops-toolbox-consul/</t>
         </is>
@@ -453,30 +463,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/global-procurement-application-designing-a-catalog-module/","Global Procurement Application: Designing a Catalog Module")</f>
         <v>0</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Sergey Derugo</t>
+        </is>
+      </c>
+      <c r="C3" s="3">
         <v>43816</v>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>2nd in a series on our Global Procurement Application (GPA) solution, discussing the cloud catalog module</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>2nd in a series on our Global Procurement Application (GPA) solution, discussing the cloud catalog module</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>Exadel Solutions</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>catalog,digital transformation,global logistics,Global Procurement Application,GPA</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>/news/global-procurement-application-designing-a-catalog-module/</t>
         </is>
@@ -487,30 +502,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/aem-tip-use-an-automated-test-framework/","AEM Tip: Use an Automated Test Framework")</f>
         <v>0</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Maryna Shantur</t>
+        </is>
+      </c>
+      <c r="C4" s="3">
         <v>43813</v>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>This tip is about the process for our team in working on AEM projects using a dialog format to present the subject of test automation.</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t xml:space="preserve">This tip is about the process for our team in working on AEM projects using a dialog format to present the subject of test automation. </t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>Tech Tips</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>AEM,automationqa,QA,qaautomation</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>/news/aem-tip-use-an-automated-test-framework/</t>
         </is>
@@ -521,30 +541,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/a-year-of-achievement-for-appery-io-in-2019/","A Year of Achievement for Appery.io in 2019")</f>
         <v>0</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Nikita Basalaev</t>
+        </is>
+      </c>
+      <c r="C5" s="3">
         <v>43810</v>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>As we look back over the year for our low-code development platform Appery.io, we have to say we are pretty proud! New features, glowing reviews...</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>As we look back over the year for our low-code development platform Appery.io, we have to say we are pretty proud! New features, glowing reviews...</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>Inside Exadel</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>Appery.io,year in review</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>/news/a-year-of-achievement-for-appery-io-in-2019/</t>
         </is>
@@ -555,30 +580,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/thats-a-wrap-2019-exadel-reflections-and-achievements/","That’s A Wrap! 2019 Exadel Reflections and Achievements")</f>
         <v>0</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Nikita Basalaev</t>
+        </is>
+      </c>
+      <c r="C6" s="3">
         <v>43804</v>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>2019 has been nothing short of exceptional! As 2019 comes to an end, we wanted to recap what made it one of the strongest years yet for Exadel.</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t xml:space="preserve">2019 has been nothing short of exceptional! As 2019 comes to an end, we wanted to recap what made it one of the strongest years yet for Exadel. </t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>Inside Exadel</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>year in review</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>/news/thats-a-wrap-2019-exadel-reflections-and-achievements/</t>
         </is>
@@ -589,30 +619,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/our-devops-methodologies-the-continuous-integration-interview/","Our DevOps Methodologies: The Continuous Integration Interview")</f>
         <v>0</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Exadel Digital Transformation Team</t>
+        </is>
+      </c>
+      <c r="C7" s="3">
         <v>43796</v>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>A conversation with Mikhail Аndrushkevich, Exadel's VP of Delivery, about the use and value of continuous integration in DevOps work</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>A conversation with Mikhail Аndrushkevich, Exadel's VP of Delivery, about the use and value of continuous integration in DevOps work</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>Development</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>continuous integration,DevOps,devopsmethodologies series,interview,series</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>/news/our-devops-methodologies-the-continuous-integration-interview/</t>
         </is>
@@ -623,30 +658,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/global-procurement-application-designing-an-inventory-module/","Global Procurement Application: Designing an Inventory Module")</f>
         <v>0</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Alexey Chumakov</t>
+        </is>
+      </c>
+      <c r="C8" s="3">
         <v>43795</v>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>1st in a series on our Global Procurement Application (GPA) solution, starting with design considerations for an inventory module</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>1st in a series on our Global Procurement Application (GPA) solution, starting with design considerations for an inventory module</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>Exadel Solutions</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>digital transformation,global logistics,Global Procurement Application,GPA,inventory,procurement,supply chain</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>/news/global-procurement-application-designing-an-inventory-module/</t>
         </is>
@@ -657,30 +697,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/aem-experience-fragments-architecture/","AEM Experience Fragments: Architecture")</f>
         <v>0</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Iryna Ason</t>
+        </is>
+      </c>
+      <c r="C9" s="3">
         <v>43784</v>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>An overview of the AEM Experience Fragment (XF) feature for the efficient organization of sections of content and presentation for use in pages</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>An overview of the AEM Experience Fragment (XF) feature for the efficient organization of sections of content and presentation for use in pages</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>Tools</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>AEM,experiencefragments,XF</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>/news/aem-experience-fragments-architecture/</t>
         </is>
@@ -691,30 +736,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/our-devops-toolbox-kubernetes/","Our DevOps Toolbox: Kubernetes")</f>
         <v>0</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Exadel Digital Transformation Team</t>
+        </is>
+      </c>
+      <c r="C10" s="3">
         <v>43766</v>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>Kubernetes is a container orchestration tool for packages of code and resources. Find out the benefits we've seen using it for development and business.</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>Kubernetes is a container orchestration tool for packages of code and resources. Find out the benefits we've seen using it for development and business.</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>Tools</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>DevOps,devopstoolbox series,digital transformation,Kubernetes,series</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>/news/our-devops-toolbox-kubernetes/</t>
         </is>
@@ -725,30 +775,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/our-devops-methods-continuous-integration/","Our DevOps Methodologies: Continuous Integration")</f>
         <v>0</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Exadel Digital Transformation Team</t>
+        </is>
+      </c>
+      <c r="C11" s="3">
         <v>43760</v>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>Continuous integration (CI) is an approach that automates the software development process. Find out the benefits we've seen for development and business.</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>Continuous integration (CI) is an approach that automates the software development process. Find out the benefits we've seen for development and business.</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>Development</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>continuous integration,DevOps,devopsmethodologies series,digital transformation,series</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>/news/our-devops-methods-continuous-integration/</t>
         </is>
@@ -759,30 +814,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/classic-to-touch-ui-migration-for-aem-page-properties/","Classic to Touch UI Migration for AEM: Page Properties")</f>
         <v>0</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Exadel Digital Marketing Technology Team</t>
+        </is>
+      </c>
+      <c r="C12" s="3">
         <v>43756</v>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>In this new installment on upgrading to the newer Touch UI in AEM, our Digital Marketing Technology team tackles the issue of Page Properties</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>In this new installment on upgrading to the newer Touch UI in Adobe Experience Manager, our Digital Marketing Technology team tackles the issue of Page Properties</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>Tech Tips</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>AEM,compatibility mode,migration,page properties,series,Touch UI</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>/news/classic-to-touch-ui-migration-for-aem-page-properties/</t>
         </is>
@@ -793,30 +853,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/classic-to-touch-ui-migration-for-aem-multifields/","Classic to Touch UI Migration for AEM: Multifields")</f>
         <v>0</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Liubou Masiuk</t>
+        </is>
+      </c>
+      <c r="C13" s="3">
         <v>43756</v>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>Our Digital Marketing Technology team's sharing of lessons learned in upgrading to the newer Touch UI in AEM focuses on multifields in this post</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>Our Digital Marketing Technology team’s sharing of lessons learned in upgrading to the newer Touch UI in AEM focuses on multifields in this post</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>Tech Tips</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>AEM,compatibility mode,migration,multifields,series,Touch UI</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>/news/classic-to-touch-ui-migration-for-aem-multifields/</t>
         </is>
@@ -827,30 +892,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/classic-to-touch-ui-migration-for-aem-more-tips-from-experience/","Classic to Touch UI Migration for AEM: More Tips from Experience")</f>
         <v>0</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Exadel Digital Marketing Technology Team</t>
+        </is>
+      </c>
+      <c r="C14" s="3">
         <v>43755</v>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>In this follow-up, our Digital Marketing Technology team shares some more detailed lessons learned in upgrading to the newer Touch UI in AEM</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>In this follow-up, our Digital Marketing Technology team shares some more detailed lessons learned in upgrading to the newer Touch UI in Adobe Experience Manager</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>Tech Tips</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>AEM,compatibility mode,migration,series,Touch UI</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>/news/classic-to-touch-ui-migration-for-aem-more-tips-from-experience/</t>
         </is>
@@ -861,30 +931,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/agile-development-for-non-products/","Agile Development for ""Non-Products""")</f>
         <v>0</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Jonathan Fries</t>
+        </is>
+      </c>
+      <c r="C15" s="3">
         <v>43750</v>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>Projects that are internal "non-products" can benefit from an agile approach and deliver great value for your organization, if adapted to the situation.</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>Projects that are internal "non-products" can benefit from an agile approach and deliver great value for your organization, if adapted to the situation.</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>Development</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>Agile development,internal projects,non-products</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>/news/agile-development-for-non-products/</t>
         </is>
@@ -895,30 +970,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/our-devops-toolbox-the-ansible-interview/","Our DevOps Toolbox: The Ansible Interview")</f>
         <v>0</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Exadel Digital Transformation Team</t>
+        </is>
+      </c>
+      <c r="C16" s="3">
         <v>43749</v>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>A conversation with Sergey Krivopshin, an Exadel DevOps engineer, about using Redhat Ansible to simplify and accelerate DevOps work</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>A conversation with Sergey Krivopshin, an Exadel DevOps engineer, about using Redhat Ansible to simplify and accelerate DevOps work</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>Tools</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>Ansible,configuration management,DevOps,devopstoolbox series,interview,series</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>/news/our-devops-toolbox-the-ansible-interview/</t>
         </is>
@@ -929,30 +1009,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/aem-experience-fragments-an-introduction/","AEM Experience Fragments: An Introduction")</f>
         <v>0</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Iryna Ason</t>
+        </is>
+      </c>
+      <c r="C17" s="3">
         <v>43746</v>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>An introduction to the AEM Experience Fragment (XF) feature for the efficient organization of sections of content and presentation for use in pages</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>An introduction to the AEM Experience Fragment (XF) feature for the efficient organization of sections of content and presentation for use in pages</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>Tools</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>AEM,experiencefragments,XF</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>/news/aem-experience-fragments-an-introduction/</t>
         </is>
@@ -963,30 +1048,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/getting-more-out-of-multi-cloud-for-the-enterprise/","Getting More out of Multi-Cloud for the Enterprise")</f>
         <v>0</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Jonathan Fries</t>
+        </is>
+      </c>
+      <c r="C18" s="3">
         <v>43746</v>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>Multi-cloud strategies have completed shifted the way enterpise IT works. With leveraging tools like CrossKube enterprises can maximize their benefits.</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>Multi-cloud strategies have completed shifted the way enterpise IT works. With leveraging tools like CrossKube enterprises can maximize their benefits.</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>Technology</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>CrossKube,Kubernetes,multi-cloud,XaaS</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>/news/getting-more-out-of-multi-cloud-for-the-enterprise/</t>
         </is>
@@ -997,30 +1087,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/beyond-building-software-agile-as-an-organization-wide-initiative/","Beyond Building Software: Agile as an Organization-Wide Initiative")</f>
         <v>0</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Jonathan Fries</t>
+        </is>
+      </c>
+      <c r="C19" s="3">
         <v>43739</v>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>The agile methodology can be expanded beyond programming to help the company as a whole become more nimble.</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>The agile methodology can be expanded beyond programming to help the company as a whole become more nimble.</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>Development</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="G19" t="inlineStr">
         <is>
           <t>Agile development</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="H19" t="inlineStr">
         <is>
           <t>/news/beyond-building-software-agile-as-an-organization-wide-initiative/</t>
         </is>
@@ -1031,25 +1126,30 @@
         <f>HYPERLINK("https://www.exadel.com/news/our-devops-toolbox-ansible/","Our DevOps Toolbox: Ansible")</f>
         <v>0</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Exadel Digital Transformation Team</t>
+        </is>
+      </c>
+      <c r="C20" s="3">
         <v>43738</v>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>Exadel significantly cuts infrastructure configuration time using Redhat Ansible. Our Digital Transformation Team explains how.</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>Exadel significantly cuts infrastructure configuration time using Redhat Ansible. Our Digital Transformation Team explains how.</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>Tools</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t>/news/our-devops-toolbox-ansible/</t>
         </is>
@@ -1060,30 +1160,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/how-to-take-advantage-of-globally-dispersed-it-teams/","How to Take Advantage of Globally Dispersed IT Teams")</f>
         <v>0</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Lev Shur</t>
+        </is>
+      </c>
+      <c r="C21" s="3">
         <v>43732</v>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>Here a few pointers on tapping Into global tech talent and managing that talent for best results from the President of Exadel Solutions.</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>Here a few pointers on tapping Into global tech talent and managing that talent for best results.</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="F21" t="inlineStr">
         <is>
           <t>Business</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="G21" t="inlineStr">
         <is>
           <t>global teams,remote collaboration</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="H21" t="inlineStr">
         <is>
           <t>/news/how-to-take-advantage-of-globally-dispersed-it-teams/</t>
         </is>
@@ -1094,30 +1199,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/introducing-the-adobe-experience-manager-authoring-toolkit/","Introducing the Adobe Experience Manager Authoring Toolkit")</f>
         <v>0</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Lev Shur</t>
+        </is>
+      </c>
+      <c r="C22" s="3">
         <v>43724</v>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>Adobe Experience Manager Authoring Toolkit is a customizable open source package for smoothly generating AEM components (XML) from Java.</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>Adobe Experience Manager Authoring Toolkit is a customizable open source package for smoothly generating AEM components (XML) from Java.</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>Development</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="G22" t="inlineStr">
         <is>
           <t>AEM,AEM Authoring Toolkit,Java,Open Source,XML</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="H22" t="inlineStr">
         <is>
           <t>/news/introducing-the-adobe-experience-manager-authoring-toolkit/</t>
         </is>
@@ -1128,30 +1238,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/women-in-stem-at-exadel-daria-rieznik-lead-qa-engineer/","Women in STEM at Exadel: Daria Rieznik, Lead QA Engineer")</f>
         <v>0</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Nikita Basalaev</t>
+        </is>
+      </c>
+      <c r="C23" s="3">
         <v>43717</v>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>Here is another installment in our series about the amazing stories, innovation, and contributions of the women in STEM jobs at Exadel.</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>Here is another installment in our series about the amazing stories, innovation, and contributions of the women in STEM jobs at Exadel.</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="F23" t="inlineStr">
         <is>
           <t>Inside Exadel</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="G23" t="inlineStr">
         <is>
           <t>women in STEM,Women in tech</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="H23" t="inlineStr">
         <is>
           <t>/news/women-in-stem-at-exadel-daria-rieznik-lead-qa-engineer/</t>
         </is>
@@ -1162,30 +1277,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/aem-tip-junit-tests-for-wcmusepojo-objects/","AEM Tip: JUnit Tests for WCMUsePojo Objects")</f>
         <v>0</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Alexander Bestsenny</t>
+        </is>
+      </c>
+      <c r="C24" s="3">
         <v>43717</v>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>This AEM tip from our Exadel Digital Marketing Technology team is all about solving the complexities of unit testing components in AEM.</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>This AEM tip from our Exadel Digital Marketing Technology team is all about solving the complexities of unit testing components in AEM.</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="F24" t="inlineStr">
         <is>
           <t>Tech Tips</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>AEM,AEM tips,junit,PowerMock,wcm.io,WCMUsePojo</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="H24" t="inlineStr">
         <is>
           <t>/news/aem-tip-junit-tests-for-wcmusepojo-objects/</t>
         </is>
@@ -1196,30 +1316,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/classic-to-touch-ui-migration-for-adobe-experience-manager/","Classic to Touch UI Migration for Adobe Experience Manager")</f>
         <v>0</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Nikita Basalaev</t>
+        </is>
+      </c>
+      <c r="C25" s="3">
         <v>43714</v>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>Our Digital Marketing Technology team shares some important lessons learned in upgrading to the newer Touch UI in Adobe Experience Manager</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>Sharing some important lessons learned in the front lines, upgrading to the newer Touch UI in Adobe Experience Manager</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="F25" t="inlineStr">
         <is>
           <t>Tech Tips</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="G25" t="inlineStr">
         <is>
           <t>AEM,author mode,CQ5,migration,series,Touch UI</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
+      <c r="H25" t="inlineStr">
         <is>
           <t>/news/classic-to-touch-ui-migration-for-adobe-experience-manager/</t>
         </is>
@@ -1230,30 +1355,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/emerging-technology-convergence-is-it-fact-or-fiction/","Emerging Technology Convergence: Is It Fact or Fiction?")</f>
         <v>0</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Lev Shur</t>
+        </is>
+      </c>
+      <c r="C26" s="3">
         <v>43714</v>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>Our Exadel Solutions President concisely discusses the extent and implications of technology convergence along with how you should approach the issue.</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="E26" t="inlineStr">
         <is>
           <t>Our Exadel Solutions President concisely discusses the extent and implications of technology convergence along with how you should approach the issue.</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="F26" t="inlineStr">
         <is>
           <t>Technology</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="G26" t="inlineStr">
         <is>
           <t>emerging technology,technology convergence</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
+      <c r="H26" t="inlineStr">
         <is>
           <t>/news/emerging-technology-convergence-is-it-fact-or-fiction/</t>
         </is>
@@ -1264,30 +1394,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/looking-behind-the-curtain-at-digital-marketing-technology-trends/","Looking Behind the Curtain at Digital Marketing Technology Trends")</f>
         <v>0</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Nikita Basalaev</t>
+        </is>
+      </c>
+      <c r="C27" s="3">
         <v>43714</v>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>Digital marketing strategy is all about harnessing massive amounts of customer data. What are the emerging technologies and tools that will help us do this?</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>Digital marketing strategy is all about harnessing a massive amount of customer and potential customer  data. What are the emerging technologies and tools that will help us do this?</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="F27" t="inlineStr">
         <is>
           <t>Technology</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr">
+      <c r="G27" t="inlineStr">
         <is>
           <t>Digital marketing,digital marketing trends</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr">
+      <c r="H27" t="inlineStr">
         <is>
           <t>/news/looking-behind-the-curtain-at-digital-marketing-technology-trends/</t>
         </is>
@@ -1298,30 +1433,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/crosskube-qa-rapid-deployment-of-environments-to-any-cloud/","CrossKube Q&amp;A: Rapid Deployment of Environments to Any Cloud")</f>
         <v>0</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Nikita Basalaev</t>
+        </is>
+      </c>
+      <c r="C28" s="3">
         <v>43705</v>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>We sat down with InData Labs CTO Alexey Tsiunchik to discuss the ways our Kubernetes deployment solution, CrossKube, can help support InData’s initiatives.</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="E28" t="inlineStr">
         <is>
           <t>We sat down with InData Labs CTO Alexey Tsiunchik to discuss the ways our Kubernetes deployment solution, CrossKube, can help support InData’s initiatives.</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="F28" t="inlineStr">
         <is>
           <t>Inside Exadel,Technology</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
+      <c r="G28" t="inlineStr">
         <is>
           <t>Alexey Tsiunchik,CrossKube,InData Labs,Kubernetes</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr">
+      <c r="H28" t="inlineStr">
         <is>
           <t>/news/crosskube-qa-rapid-deployment-of-environments-to-any-cloud/</t>
         </is>
@@ -1332,30 +1472,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/the-benefits-of-agile-software-development-and-how-to-measure-them/","The Benefits of Agile Software Development and How to Measure Them")</f>
         <v>0</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Nikita Basalaev</t>
+        </is>
+      </c>
+      <c r="C29" s="3">
         <v>43698</v>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>There are some major benefits from Agile when it comes to helping the bottom line, etc., but being able to measure these benefits can be the key to success.</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t xml:space="preserve">There are some major benefits from Agile when it comes to helping the bottom line, etc., but being able to measure these benefits can be the key to success. </t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
+      <c r="F29" t="inlineStr">
         <is>
           <t>Development</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr">
+      <c r="G29" t="inlineStr">
         <is>
           <t>agile</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
+      <c r="H29" t="inlineStr">
         <is>
           <t>/news/the-benefits-of-agile-software-development-and-how-to-measure-them/</t>
         </is>
@@ -1366,30 +1511,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/to-bet-or-not-to-bet-on-digital-transformation-3-trends-reshaping-the-gambling-industry/","To Bet or Not to Bet...on Digital Transformation: 3 Trends Reshaping the Gambling Industry")</f>
         <v>0</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Nikita Basalaev</t>
+        </is>
+      </c>
+      <c r="C30" s="3">
         <v>43698</v>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>Many industries are driving better customer experience and customer satisfaction via digital transformation. The gambling industry should be no exception.</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="E30" t="inlineStr">
         <is>
           <t>Many industries are driving better customer experience and customer satisfaction via digital transformation. The gambling industry should be no exception.</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
+      <c r="F30" t="inlineStr">
         <is>
           <t>Technology</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr">
+      <c r="G30" t="inlineStr">
         <is>
           <t>gambling,innovation</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr">
+      <c r="H30" t="inlineStr">
         <is>
           <t>/news/to-bet-or-not-to-bet-on-digital-transformation-3-trends-reshaping-the-gambling-industry/</t>
         </is>
@@ -1400,25 +1550,30 @@
         <f>HYPERLINK("https://www.exadel.com/news/digital-transformation-in-toll-road-authorities-past-%e2%80%a2-present-%e2%80%a2-future/","Digital Transformation for Toll Road Authorities: Past • Present • Future")</f>
         <v>0</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Nikita Basalaev</t>
+        </is>
+      </c>
+      <c r="C31" s="3">
         <v>43683</v>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="D31" t="inlineStr">
         <is>
           <t>How toll road systems have changed and which emerging technologies are impacting the industry now</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="E31" t="inlineStr">
         <is>
           <t>Take a look at how toll road systems have changed and which emerging technologies are impacting the industry now.</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="F31" t="inlineStr">
         <is>
           <t>Technology</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr">
+      <c r="H31" t="inlineStr">
         <is>
           <t>/news/digital-transformation-in-toll-road-authorities-past-â€¢-present-â€¢-future/</t>
         </is>
@@ -1429,30 +1584,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/women-in-stem-at-exadel-polina-antipova-delivery-manager-and-scrum-master/","Women in STEM at Exadel: Polina Antipova, Delivery Manager and Scrum Master")</f>
         <v>0</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Nikita Basalaev</t>
+        </is>
+      </c>
+      <c r="C32" s="3">
         <v>43683</v>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>Here is another installment in our series about the amazing stories, innovation, and contributions of the women in STEM jobs at Exadel.</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="E32" t="inlineStr">
         <is>
           <t>Here is another installment in our series about the amazing stories, innovation, and contributions of the women in STEM jobs at Exadel.</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
+      <c r="F32" t="inlineStr">
         <is>
           <t>Inside Exadel</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr">
+      <c r="G32" t="inlineStr">
         <is>
           <t>women in STEM,Women in tech</t>
         </is>
       </c>
-      <c r="G32" t="inlineStr">
+      <c r="H32" t="inlineStr">
         <is>
           <t>/news/women-in-stem-at-exadel-polina-antipova-delivery-manager-and-scrum-master/</t>
         </is>
@@ -1463,30 +1623,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/aem-tip-automating-verification-in-aem-author/","AEM Tip: Automating Verification in AEM Author")</f>
         <v>0</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Olga Zhuravleva</t>
+        </is>
+      </c>
+      <c r="C33" s="3">
         <v>43682</v>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="D33" t="inlineStr">
         <is>
           <t>This AEM tip from our Exadel Digital Marketing Technology team is all about using the coalesce command to make merges of slightly different data sets easier</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="E33" t="inlineStr">
         <is>
           <t>This AEM tip from our Exadel Digital Marketing Technology team is all about automated testing for the back-end authoring component.</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
+      <c r="F33" t="inlineStr">
         <is>
           <t>Tech Tips</t>
         </is>
       </c>
-      <c r="F33" t="inlineStr">
+      <c r="G33" t="inlineStr">
         <is>
           <t>AEM,AEM tips,author mode,QA</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr">
+      <c r="H33" t="inlineStr">
         <is>
           <t>/news/aem-tip-automating-verification-in-aem-author/</t>
         </is>
@@ -1497,30 +1662,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/introducing-crosskube-deploy-a-kubernetes-environment-in-any-cloud-fast/","Introducing CrossKube: Deploy a Kubernetes Environment in Any Cloud, Fast")</f>
         <v>0</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Exadel Innovations Team</t>
+        </is>
+      </c>
+      <c r="C34" s="3">
         <v>43676</v>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="D34" t="inlineStr">
         <is>
           <t>CrossKube is a culmination of years of experience and experimentation with Kubernetes deployments in the cloud.</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="E34" t="inlineStr">
         <is>
           <t>CrossKube is a culmination of years of experience and experimentation with Kubernetes deployments in the cloud.</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="F34" t="inlineStr">
         <is>
           <t>Technology</t>
         </is>
       </c>
-      <c r="F34" t="inlineStr">
+      <c r="G34" t="inlineStr">
         <is>
           <t>Cloud,CrossKube,innovation,Kubernetes</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr">
+      <c r="H34" t="inlineStr">
         <is>
           <t>/news/introducing-crosskube-deploy-a-kubernetes-environment-in-any-cloud-fast/</t>
         </is>
@@ -1531,30 +1701,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/recap-innovation-lab-2020-what-innovating-the-future-looks-like/","Recap: Innovation Lab 2020 What Innovating the Future Looks Like")</f>
         <v>0</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Exadel Innovations Team</t>
+        </is>
+      </c>
+      <c r="C35" s="3">
         <v>43663</v>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="D35" t="inlineStr">
         <is>
           <t>How are organizations testing emerging technologies while keeping their core business functioning? Innovation labs can be the answer.</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="E35" t="inlineStr">
         <is>
           <t>How are organizations testing emerging technologies while keeping their core business functioning? Innovation labs can be the answer.</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
+      <c r="F35" t="inlineStr">
         <is>
           <t>Development</t>
         </is>
       </c>
-      <c r="F35" t="inlineStr">
+      <c r="G35" t="inlineStr">
         <is>
           <t>fortune,innovation lab</t>
         </is>
       </c>
-      <c r="G35" t="inlineStr">
+      <c r="H35" t="inlineStr">
         <is>
           <t>/news/recap-innovation-lab-2020-what-innovating-the-future-looks-like/</t>
         </is>
@@ -1565,30 +1740,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/aem-tip-merging-on-fields-with-different-names/","AEM Tip: Merging on Fields with Different Names")</f>
         <v>0</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Denis Glushkov</t>
+        </is>
+      </c>
+      <c r="C36" s="3">
         <v>43662</v>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="D36" t="inlineStr">
         <is>
           <t>This AEM tip from our Exadel Digital Marketing Technology team is all about using the coalesce command to make merges of slightly different data sets easier</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="E36" t="inlineStr">
         <is>
           <t>This AEM tip from our Exadel Digital Marketing Technology team is all about using the coalesce command to make merges of slightly different data sets easier.</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
+      <c r="F36" t="inlineStr">
         <is>
           <t>Tech Tips</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr">
+      <c r="G36" t="inlineStr">
         <is>
           <t>AEM,AEM tips,explain query tool,index generator tool,sorting</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr">
+      <c r="H36" t="inlineStr">
         <is>
           <t>/news/aem-tip-merging-on-fields-with-different-names/</t>
         </is>
@@ -1599,30 +1779,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/the-impact-of-tech-advances-in-the-healthcare-industry/","The Impact of Tech Advances in the Healthcare Industry")</f>
         <v>0</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Exadel Innovations Team</t>
+        </is>
+      </c>
+      <c r="C37" s="3">
         <v>43655</v>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="D37" t="inlineStr">
         <is>
           <t>Four recent tech innovation examples in healthcare and how they are making an impact</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="E37" t="inlineStr">
         <is>
           <t>Four recent tech innovation examples in healthcare and how they are making an impact</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
+      <c r="F37" t="inlineStr">
         <is>
           <t>Technology</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr">
+      <c r="G37" t="inlineStr">
         <is>
           <t>innovation</t>
         </is>
       </c>
-      <c r="G37" t="inlineStr">
+      <c r="H37" t="inlineStr">
         <is>
           <t>/news/the-impact-of-tech-advances-in-the-healthcare-industry/</t>
         </is>
@@ -1633,30 +1818,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/women-in-stem-at-exadel-mary-frances-senior-ux-ui-designer/","Women in STEM at Exadel: Mary Frances Czarsty, Senior UX/UI Designer")</f>
         <v>0</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Exadel Innovations Team</t>
+        </is>
+      </c>
+      <c r="C38" s="3">
         <v>43655</v>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="D38" t="inlineStr">
         <is>
           <t>Here is another installment in our series about the amazing stories, innovation, and contributions of the women in STEM jobs at Exadel.</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="E38" t="inlineStr">
         <is>
           <t>Here is another installment in our series about the amazing stories, innovation, and contributions of the women in STEM jobs at Exadel.</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
+      <c r="F38" t="inlineStr">
         <is>
           <t>Inside Exadel</t>
         </is>
       </c>
-      <c r="F38" t="inlineStr">
+      <c r="G38" t="inlineStr">
         <is>
           <t>women in STEM,Women in tech</t>
         </is>
       </c>
-      <c r="G38" t="inlineStr">
+      <c r="H38" t="inlineStr">
         <is>
           <t>/news/women-in-stem-at-exadel-mary-frances-senior-ux-ui-designer/</t>
         </is>
@@ -1667,25 +1857,30 @@
         <f>HYPERLINK("https://www.exadel.com/news/how-digital-transformation-is-impacting-the-sports-and-fitness-industry/","How Digital Transformation Is Impacting the Sports and Fitness Industry")</f>
         <v>0</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Exadel Innovations Team</t>
+        </is>
+      </c>
+      <c r="C39" s="3">
         <v>43649</v>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="D39" t="inlineStr">
         <is>
           <t>The sports &amp; fitness industry has been at the forefront of technology implementation in the enterprise and capitalizing on digital transformation has provided them with great success.</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
+      <c r="E39" t="inlineStr">
         <is>
           <t>The sports &amp; fitness industry has been at the forefront of technology implementation in the enterprise and capitalizing on digital transformation has provided them with great success.</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
+      <c r="F39" t="inlineStr">
         <is>
           <t>Technology</t>
         </is>
       </c>
-      <c r="G39" t="inlineStr">
+      <c r="H39" t="inlineStr">
         <is>
           <t>/news/how-digital-transformation-is-impacting-the-sports-and-fitness-industry/</t>
         </is>
@@ -1696,30 +1891,35 @@
         <f>HYPERLINK("https://www.exadel.com/news/an-overview-of-the-innovation-lab/","An Overview of the Innovation Lab by Exadel")</f>
         <v>0</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Dmitry Binunsky</t>
+        </is>
+      </c>
+      <c r="C40" s="3">
         <v>43648</v>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="D40" t="inlineStr">
         <is>
           <t>The Innovation Lab allows companies to not waste precious resources on completed implementations of new technologies that may not have sufficient ROI.</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="E40" t="inlineStr">
         <is>
           <t>The Innovation Lab allows companies to try out implementations of new technologies to better evaluate potential ROI.</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
+      <c r="F40" t="inlineStr">
         <is>
           <t>Technology</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr">
+      <c r="G40" t="inlineStr">
         <is>
           <t>Agile development,innovation,innovation lab,low code</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr">
+      <c r="H40" t="inlineStr">
         <is>
           <t>/news/an-overview-of-the-innovation-lab/</t>
         </is>

</xml_diff>